<commit_message>
fix(catalogue): link from model to release
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/CatalogueCentralCollections.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/CatalogueCentralCollections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33285A6-38A7-4349-A72A-E90122A34625}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7682E350-5C36-2D45-9B28-95F2F24F0F28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="6" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="628">
   <si>
     <t>name</t>
   </si>
@@ -2198,7 +2198,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2283,6 +2283,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2624,13 +2626,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E080B8D-E59C-EC4A-8043-87277F816BB8}">
-  <dimension ref="A1:L134"/>
+  <dimension ref="A1:L136"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D92" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C68" sqref="C68"/>
+      <selection pane="bottomRight" activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4277,112 +4279,94 @@
         <v>400</v>
       </c>
     </row>
-    <row r="75" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="30" t="s">
+    <row r="75" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="48" t="s">
         <v>340</v>
       </c>
-      <c r="B75" s="30"/>
-      <c r="C75" s="30" t="s">
+      <c r="B75" s="48"/>
+      <c r="C75" s="48" t="s">
+        <v>622</v>
+      </c>
+      <c r="D75" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="E75" s="48"/>
+      <c r="F75" s="48" t="s">
+        <v>339</v>
+      </c>
+      <c r="G75" s="48"/>
+      <c r="H75" s="48"/>
+      <c r="I75" s="48"/>
+      <c r="J75" s="48"/>
+      <c r="K75" s="48"/>
+      <c r="L75" s="48"/>
+    </row>
+    <row r="76" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="48" t="s">
+        <v>340</v>
+      </c>
+      <c r="B76" s="48"/>
+      <c r="C76" s="48" t="s">
+        <v>333</v>
+      </c>
+      <c r="D76" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="E76" s="48"/>
+      <c r="F76" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="G76" s="48"/>
+      <c r="H76" s="48"/>
+      <c r="I76" s="48"/>
+      <c r="J76" s="48"/>
+      <c r="K76" s="48"/>
+      <c r="L76" s="48"/>
+    </row>
+    <row r="77" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="30" t="s">
+        <v>340</v>
+      </c>
+      <c r="B77" s="30"/>
+      <c r="C77" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="D75" s="30" t="s">
+      <c r="D77" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E75" s="30"/>
-      <c r="F75" s="30" t="s">
+      <c r="E77" s="30"/>
+      <c r="F77" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="G75" s="30"/>
-      <c r="H75" s="30"/>
-      <c r="I75" s="30"/>
-      <c r="J75" s="30" t="s">
+      <c r="G77" s="30"/>
+      <c r="H77" s="30"/>
+      <c r="I77" s="30"/>
+      <c r="J77" s="30" t="s">
         <v>390</v>
       </c>
-      <c r="K75" s="30"/>
-      <c r="L75" s="30" t="s">
+      <c r="K77" s="30"/>
+      <c r="L77" s="30" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="76" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="24" t="s">
+    <row r="78" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="24" t="s">
         <v>485</v>
       </c>
-      <c r="B76" s="24"/>
-      <c r="C76" s="24"/>
-      <c r="D76" s="24"/>
-      <c r="E76" s="24"/>
-      <c r="F76" s="24"/>
-      <c r="G76" s="24"/>
-      <c r="H76" s="24"/>
-      <c r="I76" s="24"/>
-      <c r="J76" s="24" t="s">
+      <c r="B78" s="24"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="24"/>
+      <c r="H78" s="24"/>
+      <c r="I78" s="24"/>
+      <c r="J78" s="24" t="s">
         <v>461</v>
       </c>
-      <c r="K76" s="24"/>
-      <c r="L76" s="24" t="s">
+      <c r="K78" s="24"/>
+      <c r="L78" s="24" t="s">
         <v>529</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="9" t="s">
-        <v>485</v>
-      </c>
-      <c r="B77" s="9"/>
-      <c r="C77" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E77" s="9">
-        <v>1</v>
-      </c>
-      <c r="F77" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="G77" s="9"/>
-      <c r="H77" s="9"/>
-      <c r="I77" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J77" s="9" t="s">
-        <v>402</v>
-      </c>
-      <c r="K77" s="9"/>
-      <c r="L77" s="9" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="9" t="s">
-        <v>485</v>
-      </c>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="D78" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E78" s="9">
-        <v>1</v>
-      </c>
-      <c r="F78" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9"/>
-      <c r="I78" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J78" s="9" t="s">
-        <v>482</v>
-      </c>
-      <c r="K78" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L78" s="9" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="79" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4391,48 +4375,60 @@
       </c>
       <c r="B79" s="9"/>
       <c r="C79" s="9" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E79" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="E79" s="9">
+        <v>1</v>
+      </c>
       <c r="F79" s="9" t="s">
-        <v>510</v>
+        <v>122</v>
       </c>
       <c r="G79" s="9"/>
       <c r="H79" s="9"/>
-      <c r="I79" s="9"/>
-      <c r="J79" s="9"/>
+      <c r="I79" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J79" s="9" t="s">
+        <v>402</v>
+      </c>
       <c r="K79" s="9"/>
       <c r="L79" s="9" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="9" t="s">
         <v>485</v>
       </c>
       <c r="B80" s="9"/>
       <c r="C80" s="9" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E80" s="9"/>
+      <c r="E80" s="9">
+        <v>1</v>
+      </c>
       <c r="F80" s="9" t="s">
-        <v>498</v>
+        <v>143</v>
       </c>
       <c r="G80" s="9"/>
       <c r="H80" s="9"/>
-      <c r="I80" s="9"/>
+      <c r="I80" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="J80" s="9" t="s">
-        <v>479</v>
-      </c>
-      <c r="K80" s="9"/>
+        <v>482</v>
+      </c>
+      <c r="K80" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="L80" s="9" t="s">
-        <v>540</v>
+        <v>515</v>
       </c>
     </row>
     <row r="81" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4441,100 +4437,90 @@
       </c>
       <c r="B81" s="9"/>
       <c r="C81" s="9" t="s">
-        <v>424</v>
+        <v>29</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E81" s="9"/>
-      <c r="F81" s="9"/>
+      <c r="F81" s="9" t="s">
+        <v>510</v>
+      </c>
       <c r="G81" s="9"/>
       <c r="H81" s="9"/>
       <c r="I81" s="9"/>
       <c r="J81" s="9"/>
       <c r="K81" s="9"/>
       <c r="L81" s="9" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="24" t="s">
-        <v>477</v>
-      </c>
-      <c r="B82" s="24"/>
-      <c r="C82" s="24"/>
-      <c r="D82" s="24"/>
-      <c r="E82" s="24"/>
-      <c r="F82" s="24"/>
-      <c r="G82" s="24"/>
-      <c r="H82" s="24"/>
-      <c r="I82" s="24"/>
-      <c r="J82" s="24" t="s">
-        <v>461</v>
-      </c>
-      <c r="K82" s="24"/>
-      <c r="L82" s="24" t="s">
-        <v>528</v>
+        <v>536</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="9" t="s">
+        <v>485</v>
+      </c>
+      <c r="B82" s="9"/>
+      <c r="C82" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="G82" s="9"/>
+      <c r="H82" s="9"/>
+      <c r="I82" s="9"/>
+      <c r="J82" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="K82" s="9"/>
+      <c r="L82" s="9" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="83" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="9" t="s">
-        <v>477</v>
+        <v>485</v>
       </c>
       <c r="B83" s="9"/>
       <c r="C83" s="9" t="s">
-        <v>109</v>
+        <v>424</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E83" s="9">
-        <v>1</v>
-      </c>
-      <c r="F83" s="9" t="s">
-        <v>122</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
       <c r="G83" s="9"/>
       <c r="H83" s="9"/>
-      <c r="I83" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J83" s="9" t="s">
-        <v>402</v>
-      </c>
+      <c r="I83" s="9"/>
+      <c r="J83" s="9"/>
       <c r="K83" s="9"/>
       <c r="L83" s="9" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="9" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="24" t="s">
         <v>477</v>
       </c>
-      <c r="B84" s="9"/>
-      <c r="C84" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="D84" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E84" s="9">
-        <v>1</v>
-      </c>
-      <c r="F84" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G84" s="9"/>
-      <c r="H84" s="9"/>
-      <c r="I84" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J84" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="K84" s="9"/>
-      <c r="L84" s="9" t="s">
-        <v>518</v>
+      <c r="B84" s="24"/>
+      <c r="C84" s="24"/>
+      <c r="D84" s="24"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="24"/>
+      <c r="H84" s="24"/>
+      <c r="I84" s="24"/>
+      <c r="J84" s="24" t="s">
+        <v>461</v>
+      </c>
+      <c r="K84" s="24"/>
+      <c r="L84" s="24" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="85" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4543,26 +4529,28 @@
       </c>
       <c r="B85" s="9"/>
       <c r="C85" s="9" t="s">
-        <v>316</v>
+        <v>109</v>
       </c>
       <c r="D85" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E85" s="9"/>
+      <c r="E85" s="9">
+        <v>1</v>
+      </c>
       <c r="F85" s="9" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="G85" s="9"/>
       <c r="H85" s="9"/>
-      <c r="I85" s="9"/>
+      <c r="I85" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="J85" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K85" s="9" t="s">
-        <v>29</v>
-      </c>
+        <v>402</v>
+      </c>
+      <c r="K85" s="9"/>
       <c r="L85" s="9" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="86" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4571,47 +4559,56 @@
       </c>
       <c r="B86" s="9"/>
       <c r="C86" s="9" t="s">
-        <v>29</v>
+        <v>321</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E86" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="E86" s="9">
+        <v>1</v>
+      </c>
       <c r="F86" s="9" t="s">
-        <v>510</v>
+        <v>27</v>
       </c>
       <c r="G86" s="9"/>
       <c r="H86" s="9"/>
-      <c r="I86" s="9"/>
-      <c r="J86" s="9"/>
+      <c r="I86" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J86" s="9" t="s">
+        <v>487</v>
+      </c>
       <c r="K86" s="9"/>
       <c r="L86" s="9" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="9" t="s">
         <v>477</v>
       </c>
       <c r="B87" s="9"/>
       <c r="C87" s="9" t="s">
-        <v>490</v>
+        <v>316</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E87" s="9"/>
       <c r="F87" s="9" t="s">
-        <v>478</v>
+        <v>143</v>
       </c>
       <c r="G87" s="9"/>
       <c r="H87" s="9"/>
+      <c r="I87" s="9"/>
       <c r="J87" s="9" t="s">
-        <v>486</v>
-      </c>
-      <c r="K87" s="9"/>
+        <v>488</v>
+      </c>
+      <c r="K87" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="L87" s="9" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="88" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4620,74 +4617,77 @@
       </c>
       <c r="B88" s="9"/>
       <c r="C88" s="9" t="s">
-        <v>587</v>
+        <v>29</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E88" s="9"/>
-      <c r="F88" s="9"/>
+      <c r="F88" s="9" t="s">
+        <v>510</v>
+      </c>
       <c r="G88" s="9"/>
       <c r="H88" s="9"/>
       <c r="I88" s="9"/>
       <c r="J88" s="9"/>
       <c r="K88" s="9"/>
       <c r="L88" s="9" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="B89" s="9"/>
+      <c r="C89" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="G89" s="9"/>
+      <c r="H89" s="9"/>
+      <c r="J89" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="K89" s="9"/>
+      <c r="L89" s="9" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="B90" s="9"/>
+      <c r="C90" s="9" t="s">
+        <v>587</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="9"/>
+      <c r="H90" s="9"/>
+      <c r="I90" s="9"/>
+      <c r="J90" s="9"/>
+      <c r="K90" s="9"/>
+      <c r="L90" s="9" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="89" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="24" t="s">
+    <row r="91" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="L89" s="24" t="s">
+      <c r="L91" s="24" t="s">
         <v>527</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C90" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D90" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E90" s="9">
-        <v>1</v>
-      </c>
-      <c r="F90" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="I90" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="L90" s="9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C91" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D91" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E91" s="9">
-        <v>1</v>
-      </c>
-      <c r="I91" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J91" s="9" t="s">
-        <v>481</v>
-      </c>
-      <c r="L91" s="9" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="92" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -4695,41 +4695,45 @@
         <v>125</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="D92" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F92" s="46" t="s">
-        <v>140</v>
-      </c>
-      <c r="J92" s="9" t="s">
-        <v>479</v>
+      <c r="E92" s="9">
+        <v>1</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="I92" s="9" t="b">
+        <v>1</v>
       </c>
       <c r="L92" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B93" s="9"/>
       <c r="C93" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E93" s="9">
         <v>1</v>
       </c>
-      <c r="D93" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E93" s="9"/>
-      <c r="F93" s="9"/>
-      <c r="G93" s="9"/>
-      <c r="H93" s="9"/>
-      <c r="I93" s="9"/>
-      <c r="J93" s="9"/>
-      <c r="K93" s="9"/>
+      <c r="I93" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J93" s="9" t="s">
+        <v>481</v>
+      </c>
       <c r="L93" s="9" t="s">
-        <v>522</v>
+        <v>130</v>
       </c>
     </row>
     <row r="94" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -4737,101 +4741,89 @@
         <v>125</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>439</v>
+        <v>24</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="F94" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="J94" s="9" t="s">
+        <v>479</v>
       </c>
       <c r="L94" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="9" t="s">
         <v>125</v>
       </c>
+      <c r="B95" s="9"/>
       <c r="C95" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D95" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="9"/>
+      <c r="H95" s="9"/>
+      <c r="I95" s="9"/>
+      <c r="J95" s="9"/>
+      <c r="K95" s="9"/>
+      <c r="L95" s="9" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="D96" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L96" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C97" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D95" s="9" t="s">
+      <c r="D97" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="L95" s="9" t="s">
+      <c r="L97" s="9" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="96" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="24" t="s">
+    <row r="98" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="24" t="s">
         <v>341</v>
       </c>
-      <c r="B96" s="24"/>
-      <c r="C96" s="24"/>
-      <c r="D96" s="24"/>
-      <c r="E96" s="24"/>
-      <c r="F96" s="24"/>
-      <c r="G96" s="24"/>
-      <c r="H96" s="24"/>
-      <c r="I96" s="24"/>
-      <c r="J96" s="24"/>
-      <c r="K96" s="24" t="s">
+      <c r="B98" s="24"/>
+      <c r="C98" s="24"/>
+      <c r="D98" s="24"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="24"/>
+      <c r="G98" s="24"/>
+      <c r="H98" s="24"/>
+      <c r="I98" s="24"/>
+      <c r="J98" s="24"/>
+      <c r="K98" s="24" t="s">
         <v>450</v>
       </c>
-      <c r="L96" s="24" t="s">
+      <c r="L98" s="24" t="s">
         <v>348</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="26" t="s">
-        <v>341</v>
-      </c>
-      <c r="B97" s="26"/>
-      <c r="C97" s="26" t="s">
-        <v>345</v>
-      </c>
-      <c r="D97" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="E97" s="26">
-        <v>1</v>
-      </c>
-      <c r="F97" s="26"/>
-      <c r="G97" s="26"/>
-      <c r="H97" s="26"/>
-      <c r="I97" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="J97" s="26"/>
-      <c r="K97" s="26" t="s">
-        <v>453</v>
-      </c>
-      <c r="L97" s="26" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="26" t="s">
-        <v>341</v>
-      </c>
-      <c r="B98" s="26"/>
-      <c r="C98" s="26" t="s">
-        <v>347</v>
-      </c>
-      <c r="D98" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="E98" s="26"/>
-      <c r="F98" s="26"/>
-      <c r="G98" s="26"/>
-      <c r="H98" s="26"/>
-      <c r="I98" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="J98" s="26"/>
-      <c r="K98" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="L98" s="26" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="99" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -4840,22 +4832,26 @@
       </c>
       <c r="B99" s="26"/>
       <c r="C99" s="26" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D99" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="E99" s="26"/>
+        <v>2</v>
+      </c>
+      <c r="E99" s="26">
+        <v>1</v>
+      </c>
       <c r="F99" s="26"/>
       <c r="G99" s="26"/>
       <c r="H99" s="26"/>
-      <c r="I99" s="26"/>
+      <c r="I99" s="26" t="b">
+        <v>1</v>
+      </c>
       <c r="J99" s="26"/>
       <c r="K99" s="26" t="s">
-        <v>433</v>
+        <v>453</v>
       </c>
       <c r="L99" s="26" t="s">
-        <v>455</v>
+        <v>351</v>
       </c>
     </row>
     <row r="100" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -4864,22 +4860,24 @@
       </c>
       <c r="B100" s="26"/>
       <c r="C100" s="26" t="s">
-        <v>198</v>
+        <v>347</v>
       </c>
       <c r="D100" s="26" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E100" s="26"/>
       <c r="F100" s="26"/>
       <c r="G100" s="26"/>
       <c r="H100" s="26"/>
-      <c r="I100" s="26"/>
+      <c r="I100" s="26" t="b">
+        <v>1</v>
+      </c>
       <c r="J100" s="26"/>
       <c r="K100" s="26" t="s">
-        <v>432</v>
+        <v>0</v>
       </c>
       <c r="L100" s="26" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="101" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -4888,10 +4886,10 @@
       </c>
       <c r="B101" s="26"/>
       <c r="C101" s="26" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="D101" s="26" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E101" s="26"/>
       <c r="F101" s="26"/>
@@ -4900,10 +4898,10 @@
       <c r="I101" s="26"/>
       <c r="J101" s="26"/>
       <c r="K101" s="26" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="L101" s="26" t="s">
-        <v>352</v>
+        <v>455</v>
       </c>
     </row>
     <row r="102" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -4912,7 +4910,7 @@
       </c>
       <c r="B102" s="26"/>
       <c r="C102" s="26" t="s">
-        <v>343</v>
+        <v>198</v>
       </c>
       <c r="D102" s="26" t="s">
         <v>4</v>
@@ -4924,10 +4922,10 @@
       <c r="I102" s="26"/>
       <c r="J102" s="26"/>
       <c r="K102" s="26" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="L102" s="26" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="103" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -4936,10 +4934,10 @@
       </c>
       <c r="B103" s="26"/>
       <c r="C103" s="26" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D103" s="26" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E103" s="26"/>
       <c r="F103" s="26"/>
@@ -4948,10 +4946,10 @@
       <c r="I103" s="26"/>
       <c r="J103" s="26"/>
       <c r="K103" s="26" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="L103" s="26" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="104" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -4960,10 +4958,10 @@
       </c>
       <c r="B104" s="26"/>
       <c r="C104" s="26" t="s">
-        <v>430</v>
+        <v>343</v>
       </c>
       <c r="D104" s="26" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E104" s="26"/>
       <c r="F104" s="26"/>
@@ -4972,10 +4970,10 @@
       <c r="I104" s="26"/>
       <c r="J104" s="26"/>
       <c r="K104" s="26" t="s">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="L104" s="26" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
     <row r="105" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -4984,10 +4982,10 @@
       </c>
       <c r="B105" s="26"/>
       <c r="C105" s="26" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D105" s="26" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E105" s="26"/>
       <c r="F105" s="26"/>
@@ -4996,10 +4994,10 @@
       <c r="I105" s="26"/>
       <c r="J105" s="26"/>
       <c r="K105" s="26" t="s">
-        <v>349</v>
+        <v>435</v>
       </c>
       <c r="L105" s="26" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="106" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -5008,7 +5006,7 @@
       </c>
       <c r="B106" s="26"/>
       <c r="C106" s="26" t="s">
-        <v>350</v>
+        <v>430</v>
       </c>
       <c r="D106" s="26" t="s">
         <v>2</v>
@@ -5020,10 +5018,10 @@
       <c r="I106" s="26"/>
       <c r="J106" s="26"/>
       <c r="K106" s="26" t="s">
-        <v>454</v>
+        <v>430</v>
       </c>
       <c r="L106" s="26" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="107" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -5032,10 +5030,10 @@
       </c>
       <c r="B107" s="26"/>
       <c r="C107" s="26" t="s">
-        <v>431</v>
+        <v>349</v>
       </c>
       <c r="D107" s="26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E107" s="26"/>
       <c r="F107" s="26"/>
@@ -5044,9 +5042,11 @@
       <c r="I107" s="26"/>
       <c r="J107" s="26"/>
       <c r="K107" s="26" t="s">
-        <v>431</v>
-      </c>
-      <c r="L107" s="26"/>
+        <v>349</v>
+      </c>
+      <c r="L107" s="26" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="108" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="26" t="s">
@@ -5054,102 +5054,90 @@
       </c>
       <c r="B108" s="26"/>
       <c r="C108" s="26" t="s">
-        <v>141</v>
+        <v>350</v>
       </c>
       <c r="D108" s="26" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E108" s="26"/>
-      <c r="F108" s="26" t="s">
-        <v>122</v>
-      </c>
+      <c r="F108" s="26"/>
       <c r="G108" s="26"/>
-      <c r="H108" s="26" t="s">
-        <v>126</v>
-      </c>
+      <c r="H108" s="26"/>
       <c r="I108" s="26"/>
       <c r="J108" s="26"/>
-      <c r="K108" s="26"/>
+      <c r="K108" s="26" t="s">
+        <v>454</v>
+      </c>
       <c r="L108" s="26" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="B109" s="26"/>
+      <c r="C109" s="26" t="s">
+        <v>431</v>
+      </c>
+      <c r="D109" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E109" s="26"/>
+      <c r="F109" s="26"/>
+      <c r="G109" s="26"/>
+      <c r="H109" s="26"/>
+      <c r="I109" s="26"/>
+      <c r="J109" s="26"/>
+      <c r="K109" s="26" t="s">
+        <v>431</v>
+      </c>
+      <c r="L109" s="26"/>
+    </row>
+    <row r="110" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="B110" s="26"/>
+      <c r="C110" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="D110" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E110" s="26"/>
+      <c r="F110" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="G110" s="26"/>
+      <c r="H110" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="I110" s="26"/>
+      <c r="J110" s="26"/>
+      <c r="K110" s="26"/>
+      <c r="L110" s="26" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="109" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="24" t="s">
+    <row r="111" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="B109" s="24"/>
-      <c r="C109" s="24"/>
-      <c r="D109" s="24"/>
-      <c r="E109" s="24"/>
-      <c r="F109" s="24"/>
-      <c r="G109" s="24"/>
-      <c r="H109" s="24"/>
-      <c r="I109" s="24"/>
-      <c r="J109" s="24" t="s">
+      <c r="B111" s="24"/>
+      <c r="C111" s="24"/>
+      <c r="D111" s="24"/>
+      <c r="E111" s="24"/>
+      <c r="F111" s="24"/>
+      <c r="G111" s="24"/>
+      <c r="H111" s="24"/>
+      <c r="I111" s="24"/>
+      <c r="J111" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="K109" s="24"/>
-      <c r="L109" s="24" t="s">
+      <c r="K111" s="24"/>
+      <c r="L111" s="24" t="s">
         <v>362</v>
-      </c>
-    </row>
-    <row r="110" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="B110" s="9"/>
-      <c r="C110" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D110" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E110" s="9">
-        <v>1</v>
-      </c>
-      <c r="F110" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="G110" s="9"/>
-      <c r="H110" s="9"/>
-      <c r="I110" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J110" s="9" t="s">
-        <v>399</v>
-      </c>
-      <c r="K110" s="9"/>
-      <c r="L110" s="9" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="111" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="B111" s="9"/>
-      <c r="C111" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="D111" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E111" s="9">
-        <v>1</v>
-      </c>
-      <c r="F111" s="9"/>
-      <c r="G111" s="9"/>
-      <c r="H111" s="9"/>
-      <c r="I111" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J111" s="9" t="s">
-        <v>396</v>
-      </c>
-      <c r="K111" s="9"/>
-      <c r="L111" s="9" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="112" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -5158,24 +5146,28 @@
       </c>
       <c r="B112" s="9"/>
       <c r="C112" s="9" t="s">
-        <v>497</v>
+        <v>109</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E112" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="E112" s="9">
+        <v>1</v>
+      </c>
       <c r="F112" s="9" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="G112" s="9"/>
       <c r="H112" s="9"/>
-      <c r="I112" s="9"/>
+      <c r="I112" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="J112" s="9" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="K112" s="9"/>
       <c r="L112" s="9" t="s">
-        <v>363</v>
+        <v>328</v>
       </c>
     </row>
     <row r="113" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -5184,24 +5176,26 @@
       </c>
       <c r="B113" s="9"/>
       <c r="C113" s="9" t="s">
-        <v>496</v>
+        <v>124</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E113" s="9"/>
-      <c r="F113" s="9" t="s">
-        <v>118</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E113" s="9">
+        <v>1</v>
+      </c>
+      <c r="F113" s="9"/>
       <c r="G113" s="9"/>
       <c r="H113" s="9"/>
-      <c r="I113" s="9"/>
+      <c r="I113" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="J113" s="9" t="s">
-        <v>464</v>
+        <v>396</v>
       </c>
       <c r="K113" s="9"/>
       <c r="L113" s="9" t="s">
-        <v>364</v>
+        <v>137</v>
       </c>
     </row>
     <row r="114" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -5210,24 +5204,24 @@
       </c>
       <c r="B114" s="9"/>
       <c r="C114" s="9" t="s">
-        <v>64</v>
+        <v>497</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="E114" s="9"/>
-      <c r="F114" s="9"/>
+      <c r="F114" s="9" t="s">
+        <v>136</v>
+      </c>
       <c r="G114" s="9"/>
       <c r="H114" s="9"/>
       <c r="I114" s="9"/>
       <c r="J114" s="9" t="s">
-        <v>386</v>
-      </c>
-      <c r="K114" s="9" t="s">
-        <v>432</v>
-      </c>
+        <v>397</v>
+      </c>
+      <c r="K114" s="9"/>
       <c r="L114" s="9" t="s">
-        <v>145</v>
+        <v>363</v>
       </c>
     </row>
     <row r="115" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -5236,124 +5230,140 @@
       </c>
       <c r="B115" s="9"/>
       <c r="C115" s="9" t="s">
-        <v>1</v>
+        <v>496</v>
       </c>
       <c r="D115" s="9" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E115" s="9"/>
-      <c r="F115" s="9"/>
+      <c r="F115" s="9" t="s">
+        <v>118</v>
+      </c>
       <c r="G115" s="9"/>
       <c r="H115" s="9"/>
       <c r="I115" s="9"/>
       <c r="J115" s="9" t="s">
-        <v>384</v>
+        <v>464</v>
       </c>
       <c r="K115" s="9"/>
       <c r="L115" s="9" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="B116" s="9"/>
+      <c r="C116" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D116" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E116" s="9"/>
+      <c r="F116" s="9"/>
+      <c r="G116" s="9"/>
+      <c r="H116" s="9"/>
+      <c r="I116" s="9"/>
+      <c r="J116" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="K116" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="L116" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="B117" s="9"/>
+      <c r="C117" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D117" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E117" s="9"/>
+      <c r="F117" s="9"/>
+      <c r="G117" s="9"/>
+      <c r="H117" s="9"/>
+      <c r="I117" s="9"/>
+      <c r="J117" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="K117" s="9"/>
+      <c r="L117" s="9" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="116" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="28" t="s">
+    <row r="118" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="L116" s="28" t="s">
+      <c r="L118" s="28" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="117" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C117" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D117" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E117" s="8">
-        <v>1</v>
-      </c>
-      <c r="F117" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="I117" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C118" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D118" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E118" s="8">
-        <v>1</v>
-      </c>
-      <c r="I118" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B119" s="8"/>
       <c r="C119" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D119" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E119" s="8">
         <v>1</v>
       </c>
-      <c r="D119" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E119" s="8"/>
-      <c r="F119" s="8"/>
-      <c r="G119" s="8"/>
-      <c r="H119" s="8"/>
-      <c r="I119" s="8"/>
-      <c r="J119" s="8"/>
-      <c r="K119" s="8"/>
-      <c r="L119" s="8"/>
-    </row>
-    <row r="120" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F119" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="I119" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B120" s="8"/>
       <c r="C120" s="8" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E120" s="8"/>
-      <c r="F120" s="8"/>
-      <c r="G120" s="8"/>
-      <c r="H120" s="8"/>
-      <c r="I120" s="8"/>
-      <c r="J120" s="8"/>
-      <c r="K120" s="8"/>
-      <c r="L120" s="8" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="121" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="E120" s="8">
+        <v>1</v>
+      </c>
+      <c r="I120" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="B121" s="8"/>
       <c r="C121" s="8" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="L121" s="8" t="s">
-        <v>371</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E121" s="8"/>
+      <c r="F121" s="8"/>
+      <c r="G121" s="8"/>
+      <c r="H121" s="8"/>
+      <c r="I121" s="8"/>
+      <c r="J121" s="8"/>
+      <c r="K121" s="8"/>
+      <c r="L121" s="8"/>
     </row>
     <row r="122" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="8" t="s">
@@ -5361,46 +5371,34 @@
       </c>
       <c r="B122" s="8"/>
       <c r="C122" s="8" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E122" s="8"/>
-      <c r="F122" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="F122" s="8"/>
       <c r="G122" s="8"/>
       <c r="H122" s="8"/>
       <c r="I122" s="8"/>
       <c r="J122" s="8"/>
       <c r="K122" s="8"/>
       <c r="L122" s="8" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B123" s="8"/>
       <c r="C123" s="8" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E123" s="8"/>
-      <c r="F123" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G123" s="8"/>
-      <c r="H123" s="8"/>
-      <c r="I123" s="8"/>
-      <c r="J123" s="8"/>
-      <c r="K123" s="8"/>
+        <v>4</v>
+      </c>
       <c r="L123" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="124" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -5409,20 +5407,22 @@
       </c>
       <c r="B124" s="8"/>
       <c r="C124" s="8" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E124" s="8"/>
-      <c r="F124" s="8"/>
+      <c r="F124" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="G124" s="8"/>
       <c r="H124" s="8"/>
       <c r="I124" s="8"/>
       <c r="J124" s="8"/>
       <c r="K124" s="8"/>
       <c r="L124" s="8" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="125" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -5431,36 +5431,34 @@
       </c>
       <c r="B125" s="8"/>
       <c r="C125" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E125" s="8"/>
       <c r="F125" s="8" t="s">
-        <v>491</v>
-      </c>
-      <c r="G125" s="8" t="s">
-        <v>109</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G125" s="8"/>
       <c r="H125" s="8"/>
       <c r="I125" s="8"/>
       <c r="J125" s="8"/>
       <c r="K125" s="8"/>
       <c r="L125" s="8" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="126" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B126" s="8"/>
       <c r="C126" s="8" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E126" s="8"/>
       <c r="F126" s="8"/>
@@ -5470,72 +5468,66 @@
       <c r="J126" s="8"/>
       <c r="K126" s="8"/>
       <c r="L126" s="8" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="127" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B127" s="8"/>
+      <c r="C127" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D127" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E127" s="8"/>
+      <c r="F127" s="8" t="s">
         <v>491</v>
       </c>
-      <c r="K127" s="28" t="s">
-        <v>446</v>
-      </c>
-      <c r="L127" s="28" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="128" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G127" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H127" s="8"/>
+      <c r="I127" s="8"/>
+      <c r="J127" s="8"/>
+      <c r="K127" s="8"/>
+      <c r="L127" s="8" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="8" t="s">
-        <v>491</v>
+        <v>19</v>
       </c>
       <c r="B128" s="8"/>
       <c r="C128" s="8" t="s">
-        <v>109</v>
+        <v>44</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E128" s="8">
-        <v>1</v>
-      </c>
-      <c r="F128" s="8" t="s">
-        <v>122</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E128" s="8"/>
+      <c r="F128" s="8"/>
       <c r="G128" s="8"/>
       <c r="H128" s="8"/>
-      <c r="I128" s="8" t="b">
-        <v>1</v>
-      </c>
+      <c r="I128" s="8"/>
       <c r="J128" s="8"/>
       <c r="K128" s="8"/>
       <c r="L128" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="129" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="8" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="28" t="s">
         <v>491</v>
       </c>
-      <c r="B129" s="8"/>
-      <c r="C129" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D129" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E129" s="8">
-        <v>1</v>
-      </c>
-      <c r="F129" s="8"/>
-      <c r="G129" s="8"/>
-      <c r="H129" s="8"/>
-      <c r="I129" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="J129" s="8"/>
-      <c r="K129" s="8"/>
-      <c r="L129" s="8" t="s">
-        <v>6</v>
+      <c r="K129" s="28" t="s">
+        <v>446</v>
+      </c>
+      <c r="L129" s="28" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="130" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -5544,19 +5536,27 @@
       </c>
       <c r="B130" s="8"/>
       <c r="C130" s="8" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E130" s="8"/>
-      <c r="F130" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="E130" s="8">
+        <v>1</v>
+      </c>
+      <c r="F130" s="8" t="s">
+        <v>122</v>
+      </c>
       <c r="G130" s="8"/>
       <c r="H130" s="8"/>
-      <c r="I130" s="8"/>
+      <c r="I130" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="J130" s="8"/>
       <c r="K130" s="8"/>
-      <c r="L130" s="8"/>
+      <c r="L130" s="8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="131" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="8" t="s">
@@ -5564,64 +5564,110 @@
       </c>
       <c r="B131" s="8"/>
       <c r="C131" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D131" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E131" s="8">
         <v>1</v>
       </c>
-      <c r="D131" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E131" s="8"/>
       <c r="F131" s="8"/>
       <c r="G131" s="8"/>
       <c r="H131" s="8"/>
-      <c r="I131" s="8"/>
+      <c r="I131" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="J131" s="8"/>
       <c r="K131" s="8"/>
-      <c r="L131" s="8"/>
-    </row>
-    <row r="132" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L131" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="8" t="s">
         <v>491</v>
       </c>
+      <c r="B132" s="8"/>
       <c r="C132" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F132" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="133" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="E132" s="8"/>
+      <c r="F132" s="8"/>
+      <c r="G132" s="8"/>
+      <c r="H132" s="8"/>
+      <c r="I132" s="8"/>
+      <c r="J132" s="8"/>
+      <c r="K132" s="8"/>
+      <c r="L132" s="8"/>
+    </row>
+    <row r="133" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A133" s="8" t="s">
         <v>491</v>
       </c>
+      <c r="B133" s="8"/>
       <c r="C133" s="8" t="s">
-        <v>493</v>
+        <v>1</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F133" s="8" t="s">
-        <v>561</v>
-      </c>
-      <c r="L133" s="8" t="s">
-        <v>98</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E133" s="8"/>
+      <c r="F133" s="8"/>
+      <c r="G133" s="8"/>
+      <c r="H133" s="8"/>
+      <c r="I133" s="8"/>
+      <c r="J133" s="8"/>
+      <c r="K133" s="8"/>
+      <c r="L133" s="8"/>
     </row>
     <row r="134" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="8" t="s">
         <v>491</v>
       </c>
       <c r="C134" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D134" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F134" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="C135" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="D135" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F135" s="8" t="s">
+        <v>561</v>
+      </c>
+      <c r="L135" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="C136" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D134" s="8" t="s">
+      <c r="D136" s="8" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M95" xr:uid="{05A83487-31A5-894A-B1C5-9D57C8ECFC86}"/>
+  <autoFilter ref="A1:M97" xr:uid="{05A83487-31A5-894A-B1C5-9D57C8ECFC86}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -8359,7 +8405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89AD2AFD-13A0-5345-A70A-10CB56C80F1B}">
   <dimension ref="E1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat(semantics): refactored linked data system, the magic attribute is now called 'semantics' and can now also be labeled 'id' which means it will be used as IRI for references (typical use case: ontology terms)
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/CatalogueCentralCollections.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/CatalogueCentralCollections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7682E350-5C36-2D45-9B28-95F2F24F0F28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C151E31-ED40-5347-AC94-8222300D41CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="628">
   <si>
     <t>name</t>
   </si>
@@ -2198,7 +2198,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2285,6 +2285,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2626,13 +2629,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E080B8D-E59C-EC4A-8043-87277F816BB8}">
-  <dimension ref="A1:L136"/>
+  <dimension ref="A1:L139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F76" sqref="F76"/>
+      <selection pane="bottomRight" activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4184,33 +4187,32 @@
       <c r="K70" s="31"/>
       <c r="L70" s="31"/>
     </row>
-    <row r="71" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="31" t="s">
+    <row r="71" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="48" t="s">
+        <v>338</v>
+      </c>
+      <c r="B71" s="30"/>
+      <c r="C71" s="30" t="s">
+        <v>622</v>
+      </c>
+      <c r="D71" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E71" s="30"/>
+      <c r="F71" s="30" t="s">
         <v>339</v>
       </c>
-      <c r="B71" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="C71" s="31"/>
-      <c r="D71" s="31"/>
-      <c r="E71" s="31"/>
-      <c r="F71" s="31"/>
-      <c r="G71" s="31"/>
-      <c r="H71" s="31"/>
-      <c r="I71" s="31"/>
-      <c r="J71" s="31" t="s">
-        <v>381</v>
-      </c>
-      <c r="K71" s="31" t="s">
-        <v>448</v>
-      </c>
-      <c r="L71" s="31" t="s">
-        <v>421</v>
-      </c>
+      <c r="G71" s="30"/>
+      <c r="H71" s="30"/>
+      <c r="I71" s="30"/>
+      <c r="J71" s="30" t="s">
+        <v>390</v>
+      </c>
+      <c r="L71" s="30"/>
     </row>
     <row r="72" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="30" t="s">
-        <v>339</v>
+      <c r="A72" s="48" t="s">
+        <v>338</v>
       </c>
       <c r="B72" s="30"/>
       <c r="C72" s="30" t="s">
@@ -4232,8 +4234,8 @@
       <c r="L72" s="30"/>
     </row>
     <row r="73" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="30" t="s">
-        <v>339</v>
+      <c r="A73" s="48" t="s">
+        <v>338</v>
       </c>
       <c r="B73" s="30"/>
       <c r="C73" s="30" t="s">
@@ -4257,7 +4259,7 @@
     </row>
     <row r="74" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B74" s="31" t="s">
         <v>122</v>
@@ -4270,215 +4272,204 @@
       <c r="H74" s="31"/>
       <c r="I74" s="31"/>
       <c r="J74" s="31" t="s">
+        <v>381</v>
+      </c>
+      <c r="K74" s="31" t="s">
+        <v>448</v>
+      </c>
+      <c r="L74" s="31" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="30" t="s">
+        <v>339</v>
+      </c>
+      <c r="B75" s="30"/>
+      <c r="C75" s="30" t="s">
+        <v>333</v>
+      </c>
+      <c r="D75" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E75" s="30"/>
+      <c r="F75" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="G75" s="30"/>
+      <c r="H75" s="30"/>
+      <c r="I75" s="30"/>
+      <c r="J75" s="30" t="s">
+        <v>390</v>
+      </c>
+      <c r="L75" s="30"/>
+    </row>
+    <row r="76" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="30" t="s">
+        <v>339</v>
+      </c>
+      <c r="B76" s="30"/>
+      <c r="C76" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="D76" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E76" s="30"/>
+      <c r="F76" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="G76" s="30"/>
+      <c r="H76" s="30"/>
+      <c r="I76" s="30"/>
+      <c r="J76" s="30" t="s">
+        <v>390</v>
+      </c>
+      <c r="K76" s="30"/>
+      <c r="L76" s="30"/>
+    </row>
+    <row r="77" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="31" t="s">
+        <v>340</v>
+      </c>
+      <c r="B77" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="C77" s="31"/>
+      <c r="D77" s="31"/>
+      <c r="E77" s="31"/>
+      <c r="F77" s="31"/>
+      <c r="G77" s="31"/>
+      <c r="H77" s="31"/>
+      <c r="I77" s="31"/>
+      <c r="J77" s="31" t="s">
         <v>456</v>
       </c>
-      <c r="K74" s="31" t="s">
+      <c r="K77" s="31" t="s">
         <v>451</v>
       </c>
-      <c r="L74" s="31" t="s">
+      <c r="L77" s="31" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="75" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="48" t="s">
+    <row r="78" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="48" t="s">
         <v>340</v>
       </c>
-      <c r="B75" s="48"/>
-      <c r="C75" s="48" t="s">
+      <c r="B78" s="48"/>
+      <c r="C78" s="48" t="s">
         <v>622</v>
       </c>
-      <c r="D75" s="48" t="s">
+      <c r="D78" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="E75" s="48"/>
-      <c r="F75" s="48" t="s">
+      <c r="E78" s="48"/>
+      <c r="F78" s="48" t="s">
         <v>339</v>
       </c>
-      <c r="G75" s="48"/>
-      <c r="H75" s="48"/>
-      <c r="I75" s="48"/>
-      <c r="J75" s="48"/>
-      <c r="K75" s="48"/>
-      <c r="L75" s="48"/>
-    </row>
-    <row r="76" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="48" t="s">
+      <c r="G78" s="48"/>
+      <c r="H78" s="48"/>
+      <c r="I78" s="48"/>
+      <c r="J78" s="48"/>
+      <c r="K78" s="48"/>
+      <c r="L78" s="48"/>
+    </row>
+    <row r="79" spans="1:12" s="49" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="48" t="s">
         <v>340</v>
       </c>
-      <c r="B76" s="48"/>
-      <c r="C76" s="48" t="s">
+      <c r="B79" s="48"/>
+      <c r="C79" s="48" t="s">
         <v>333</v>
       </c>
-      <c r="D76" s="48" t="s">
+      <c r="D79" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="E76" s="48"/>
-      <c r="F76" s="48" t="s">
+      <c r="E79" s="48"/>
+      <c r="F79" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="G76" s="48"/>
-      <c r="H76" s="48"/>
-      <c r="I76" s="48"/>
-      <c r="J76" s="48"/>
-      <c r="K76" s="48"/>
-      <c r="L76" s="48"/>
-    </row>
-    <row r="77" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="30" t="s">
+      <c r="G79" s="48"/>
+      <c r="H79" s="48"/>
+      <c r="I79" s="48"/>
+      <c r="J79" s="48"/>
+      <c r="K79" s="48"/>
+      <c r="L79" s="48"/>
+    </row>
+    <row r="80" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="30" t="s">
         <v>340</v>
       </c>
-      <c r="B77" s="30"/>
-      <c r="C77" s="30" t="s">
+      <c r="B80" s="30"/>
+      <c r="C80" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="D77" s="30" t="s">
+      <c r="D80" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E77" s="30"/>
-      <c r="F77" s="30" t="s">
+      <c r="E80" s="30"/>
+      <c r="F80" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="G77" s="30"/>
-      <c r="H77" s="30"/>
-      <c r="I77" s="30"/>
-      <c r="J77" s="30" t="s">
+      <c r="G80" s="30"/>
+      <c r="H80" s="30"/>
+      <c r="I80" s="30"/>
+      <c r="J80" s="30" t="s">
         <v>390</v>
       </c>
-      <c r="K77" s="30"/>
-      <c r="L77" s="30" t="s">
+      <c r="K80" s="30"/>
+      <c r="L80" s="30" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="78" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="24" t="s">
+    <row r="81" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="24" t="s">
         <v>485</v>
       </c>
-      <c r="B78" s="24"/>
-      <c r="C78" s="24"/>
-      <c r="D78" s="24"/>
-      <c r="E78" s="24"/>
-      <c r="F78" s="24"/>
-      <c r="G78" s="24"/>
-      <c r="H78" s="24"/>
-      <c r="I78" s="24"/>
-      <c r="J78" s="24" t="s">
+      <c r="B81" s="24"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="24"/>
+      <c r="H81" s="24"/>
+      <c r="I81" s="24"/>
+      <c r="J81" s="24" t="s">
         <v>461</v>
       </c>
-      <c r="K78" s="24"/>
-      <c r="L78" s="24" t="s">
+      <c r="K81" s="24"/>
+      <c r="L81" s="24" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="79" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="9" t="s">
-        <v>485</v>
-      </c>
-      <c r="B79" s="9"/>
-      <c r="C79" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E79" s="9">
-        <v>1</v>
-      </c>
-      <c r="F79" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="G79" s="9"/>
-      <c r="H79" s="9"/>
-      <c r="I79" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J79" s="9" t="s">
-        <v>402</v>
-      </c>
-      <c r="K79" s="9"/>
-      <c r="L79" s="9" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="9" t="s">
-        <v>485</v>
-      </c>
-      <c r="B80" s="9"/>
-      <c r="C80" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="D80" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E80" s="9">
-        <v>1</v>
-      </c>
-      <c r="F80" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="G80" s="9"/>
-      <c r="H80" s="9"/>
-      <c r="I80" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J80" s="9" t="s">
-        <v>482</v>
-      </c>
-      <c r="K80" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L80" s="9" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="9" t="s">
-        <v>485</v>
-      </c>
-      <c r="B81" s="9"/>
-      <c r="C81" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E81" s="9"/>
-      <c r="F81" s="9" t="s">
-        <v>510</v>
-      </c>
-      <c r="G81" s="9"/>
-      <c r="H81" s="9"/>
-      <c r="I81" s="9"/>
-      <c r="J81" s="9"/>
-      <c r="K81" s="9"/>
-      <c r="L81" s="9" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="9" t="s">
         <v>485</v>
       </c>
       <c r="B82" s="9"/>
       <c r="C82" s="9" t="s">
-        <v>320</v>
+        <v>109</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E82" s="9"/>
+      <c r="E82" s="9">
+        <v>1</v>
+      </c>
       <c r="F82" s="9" t="s">
-        <v>498</v>
+        <v>122</v>
       </c>
       <c r="G82" s="9"/>
       <c r="H82" s="9"/>
-      <c r="I82" s="9"/>
+      <c r="I82" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="J82" s="9" t="s">
-        <v>479</v>
+        <v>402</v>
       </c>
       <c r="K82" s="9"/>
       <c r="L82" s="9" t="s">
-        <v>540</v>
+        <v>517</v>
       </c>
     </row>
     <row r="83" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4487,128 +4478,122 @@
       </c>
       <c r="B83" s="9"/>
       <c r="C83" s="9" t="s">
-        <v>424</v>
+        <v>316</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E83" s="9"/>
-      <c r="F83" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="E83" s="9">
+        <v>1</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>143</v>
+      </c>
       <c r="G83" s="9"/>
       <c r="H83" s="9"/>
-      <c r="I83" s="9"/>
-      <c r="J83" s="9"/>
-      <c r="K83" s="9"/>
+      <c r="I83" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J83" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="K83" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="L83" s="9" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="24" t="s">
-        <v>477</v>
-      </c>
-      <c r="B84" s="24"/>
-      <c r="C84" s="24"/>
-      <c r="D84" s="24"/>
-      <c r="E84" s="24"/>
-      <c r="F84" s="24"/>
-      <c r="G84" s="24"/>
-      <c r="H84" s="24"/>
-      <c r="I84" s="24"/>
-      <c r="J84" s="24" t="s">
-        <v>461</v>
-      </c>
-      <c r="K84" s="24"/>
-      <c r="L84" s="24" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="9" t="s">
+        <v>485</v>
+      </c>
+      <c r="B84" s="9"/>
+      <c r="C84" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D84" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="G84" s="9"/>
+      <c r="H84" s="9"/>
+      <c r="I84" s="9"/>
+      <c r="J84" s="9"/>
+      <c r="K84" s="9"/>
+      <c r="L84" s="9" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="9" t="s">
-        <v>477</v>
+        <v>485</v>
       </c>
       <c r="B85" s="9"/>
       <c r="C85" s="9" t="s">
-        <v>109</v>
+        <v>320</v>
       </c>
       <c r="D85" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E85" s="9">
-        <v>1</v>
-      </c>
+      <c r="E85" s="9"/>
       <c r="F85" s="9" t="s">
-        <v>122</v>
+        <v>498</v>
       </c>
       <c r="G85" s="9"/>
       <c r="H85" s="9"/>
-      <c r="I85" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="I85" s="9"/>
       <c r="J85" s="9" t="s">
-        <v>402</v>
+        <v>479</v>
       </c>
       <c r="K85" s="9"/>
       <c r="L85" s="9" t="s">
-        <v>516</v>
+        <v>540</v>
       </c>
     </row>
     <row r="86" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="9" t="s">
-        <v>477</v>
+        <v>485</v>
       </c>
       <c r="B86" s="9"/>
       <c r="C86" s="9" t="s">
-        <v>321</v>
+        <v>424</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E86" s="9">
-        <v>1</v>
-      </c>
-      <c r="F86" s="9" t="s">
-        <v>27</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
       <c r="G86" s="9"/>
       <c r="H86" s="9"/>
-      <c r="I86" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J86" s="9" t="s">
-        <v>487</v>
-      </c>
+      <c r="I86" s="9"/>
+      <c r="J86" s="9"/>
       <c r="K86" s="9"/>
       <c r="L86" s="9" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="9" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="24" t="s">
         <v>477</v>
       </c>
-      <c r="B87" s="9"/>
-      <c r="C87" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="D87" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E87" s="9"/>
-      <c r="F87" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="G87" s="9"/>
-      <c r="H87" s="9"/>
-      <c r="I87" s="9"/>
-      <c r="J87" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="K87" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L87" s="9" t="s">
-        <v>519</v>
+      <c r="B87" s="24"/>
+      <c r="C87" s="24"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="24"/>
+      <c r="H87" s="24"/>
+      <c r="I87" s="24"/>
+      <c r="J87" s="24" t="s">
+        <v>461</v>
+      </c>
+      <c r="K87" s="24"/>
+      <c r="L87" s="24" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="88" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4617,47 +4602,58 @@
       </c>
       <c r="B88" s="9"/>
       <c r="C88" s="9" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E88" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="E88" s="9">
+        <v>1</v>
+      </c>
       <c r="F88" s="9" t="s">
-        <v>510</v>
+        <v>122</v>
       </c>
       <c r="G88" s="9"/>
       <c r="H88" s="9"/>
-      <c r="I88" s="9"/>
-      <c r="J88" s="9"/>
+      <c r="I88" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J88" s="9" t="s">
+        <v>402</v>
+      </c>
       <c r="K88" s="9"/>
       <c r="L88" s="9" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="9" t="s">
         <v>477</v>
       </c>
       <c r="B89" s="9"/>
       <c r="C89" s="9" t="s">
-        <v>490</v>
+        <v>321</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E89" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="E89" s="9">
+        <v>1</v>
+      </c>
       <c r="F89" s="9" t="s">
-        <v>478</v>
+        <v>27</v>
       </c>
       <c r="G89" s="9"/>
       <c r="H89" s="9"/>
+      <c r="I89" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="J89" s="9" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="K89" s="9"/>
       <c r="L89" s="9" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="90" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4666,116 +4662,128 @@
       </c>
       <c r="B90" s="9"/>
       <c r="C90" s="9" t="s">
-        <v>587</v>
+        <v>316</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E90" s="9"/>
-      <c r="F90" s="9"/>
+      <c r="F90" s="9" t="s">
+        <v>143</v>
+      </c>
       <c r="G90" s="9"/>
       <c r="H90" s="9"/>
       <c r="I90" s="9"/>
-      <c r="J90" s="9"/>
-      <c r="K90" s="9"/>
+      <c r="J90" s="9" t="s">
+        <v>488</v>
+      </c>
+      <c r="K90" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="L90" s="9" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="B91" s="9"/>
+      <c r="C91" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="G91" s="9"/>
+      <c r="H91" s="9"/>
+      <c r="I91" s="9"/>
+      <c r="J91" s="9"/>
+      <c r="K91" s="9"/>
+      <c r="L91" s="9" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="B92" s="9"/>
+      <c r="C92" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="G92" s="9"/>
+      <c r="H92" s="9"/>
+      <c r="J92" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="K92" s="9"/>
+      <c r="L92" s="9" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="B93" s="9"/>
+      <c r="C93" s="9" t="s">
+        <v>587</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="9"/>
+      <c r="H93" s="9"/>
+      <c r="I93" s="9"/>
+      <c r="J93" s="9"/>
+      <c r="K93" s="9"/>
+      <c r="L93" s="9" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="91" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="24" t="s">
+    <row r="94" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="L91" s="24" t="s">
+      <c r="L94" s="24" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="92" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C92" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D92" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E92" s="9">
-        <v>1</v>
-      </c>
-      <c r="F92" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="I92" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="L92" s="9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C93" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D93" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E93" s="9">
-        <v>1</v>
-      </c>
-      <c r="I93" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J93" s="9" t="s">
-        <v>481</v>
-      </c>
-      <c r="L93" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C94" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D94" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F94" s="46" t="s">
-        <v>140</v>
-      </c>
-      <c r="J94" s="9" t="s">
-        <v>479</v>
-      </c>
-      <c r="L94" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B95" s="9"/>
       <c r="C95" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D95" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E95" s="9">
         <v>1</v>
       </c>
-      <c r="D95" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E95" s="9"/>
-      <c r="F95" s="9"/>
-      <c r="G95" s="9"/>
-      <c r="H95" s="9"/>
-      <c r="I95" s="9"/>
-      <c r="J95" s="9"/>
-      <c r="K95" s="9"/>
+      <c r="F95" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="I95" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="L95" s="9" t="s">
-        <v>522</v>
+        <v>127</v>
       </c>
     </row>
     <row r="96" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -4783,13 +4791,22 @@
         <v>125</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>439</v>
+        <v>0</v>
       </c>
       <c r="D96" s="9" t="s">
         <v>2</v>
       </c>
+      <c r="E96" s="9">
+        <v>1</v>
+      </c>
+      <c r="I96" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J96" s="9" t="s">
+        <v>481</v>
+      </c>
       <c r="L96" s="9" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="97" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -4797,111 +4814,89 @@
         <v>125</v>
       </c>
       <c r="C97" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D97" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F97" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="J97" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="L97" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B98" s="9"/>
+      <c r="C98" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D98" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E98" s="9"/>
+      <c r="F98" s="9"/>
+      <c r="G98" s="9"/>
+      <c r="H98" s="9"/>
+      <c r="I98" s="9"/>
+      <c r="J98" s="9"/>
+      <c r="K98" s="9"/>
+      <c r="L98" s="9" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L99" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C100" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D97" s="9" t="s">
+      <c r="D100" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="L97" s="9" t="s">
+      <c r="L100" s="9" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="98" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="24" t="s">
+    <row r="101" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="24" t="s">
         <v>341</v>
       </c>
-      <c r="B98" s="24"/>
-      <c r="C98" s="24"/>
-      <c r="D98" s="24"/>
-      <c r="E98" s="24"/>
-      <c r="F98" s="24"/>
-      <c r="G98" s="24"/>
-      <c r="H98" s="24"/>
-      <c r="I98" s="24"/>
-      <c r="J98" s="24"/>
-      <c r="K98" s="24" t="s">
+      <c r="B101" s="24"/>
+      <c r="C101" s="24"/>
+      <c r="D101" s="24"/>
+      <c r="E101" s="24"/>
+      <c r="F101" s="24"/>
+      <c r="G101" s="24"/>
+      <c r="H101" s="24"/>
+      <c r="I101" s="24"/>
+      <c r="J101" s="24"/>
+      <c r="K101" s="24" t="s">
         <v>450</v>
       </c>
-      <c r="L98" s="24" t="s">
+      <c r="L101" s="24" t="s">
         <v>348</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="26" t="s">
-        <v>341</v>
-      </c>
-      <c r="B99" s="26"/>
-      <c r="C99" s="26" t="s">
-        <v>345</v>
-      </c>
-      <c r="D99" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="E99" s="26">
-        <v>1</v>
-      </c>
-      <c r="F99" s="26"/>
-      <c r="G99" s="26"/>
-      <c r="H99" s="26"/>
-      <c r="I99" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="J99" s="26"/>
-      <c r="K99" s="26" t="s">
-        <v>453</v>
-      </c>
-      <c r="L99" s="26" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="26" t="s">
-        <v>341</v>
-      </c>
-      <c r="B100" s="26"/>
-      <c r="C100" s="26" t="s">
-        <v>347</v>
-      </c>
-      <c r="D100" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="E100" s="26"/>
-      <c r="F100" s="26"/>
-      <c r="G100" s="26"/>
-      <c r="H100" s="26"/>
-      <c r="I100" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="J100" s="26"/>
-      <c r="K100" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="L100" s="26" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="26" t="s">
-        <v>341</v>
-      </c>
-      <c r="B101" s="26"/>
-      <c r="C101" s="26" t="s">
-        <v>344</v>
-      </c>
-      <c r="D101" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="E101" s="26"/>
-      <c r="F101" s="26"/>
-      <c r="G101" s="26"/>
-      <c r="H101" s="26"/>
-      <c r="I101" s="26"/>
-      <c r="J101" s="26"/>
-      <c r="K101" s="26" t="s">
-        <v>433</v>
-      </c>
-      <c r="L101" s="26" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="102" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -4910,22 +4905,26 @@
       </c>
       <c r="B102" s="26"/>
       <c r="C102" s="26" t="s">
-        <v>198</v>
+        <v>345</v>
       </c>
       <c r="D102" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="E102" s="26"/>
+        <v>2</v>
+      </c>
+      <c r="E102" s="26">
+        <v>1</v>
+      </c>
       <c r="F102" s="26"/>
       <c r="G102" s="26"/>
       <c r="H102" s="26"/>
-      <c r="I102" s="26"/>
+      <c r="I102" s="26" t="b">
+        <v>1</v>
+      </c>
       <c r="J102" s="26"/>
       <c r="K102" s="26" t="s">
-        <v>432</v>
+        <v>453</v>
       </c>
       <c r="L102" s="26" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
     </row>
     <row r="103" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -4934,7 +4933,7 @@
       </c>
       <c r="B103" s="26"/>
       <c r="C103" s="26" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="D103" s="26" t="s">
         <v>2</v>
@@ -4943,13 +4942,15 @@
       <c r="F103" s="26"/>
       <c r="G103" s="26"/>
       <c r="H103" s="26"/>
-      <c r="I103" s="26"/>
+      <c r="I103" s="26" t="b">
+        <v>1</v>
+      </c>
       <c r="J103" s="26"/>
       <c r="K103" s="26" t="s">
-        <v>434</v>
+        <v>0</v>
       </c>
       <c r="L103" s="26" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
     </row>
     <row r="104" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -4958,10 +4959,10 @@
       </c>
       <c r="B104" s="26"/>
       <c r="C104" s="26" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D104" s="26" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E104" s="26"/>
       <c r="F104" s="26"/>
@@ -4970,10 +4971,10 @@
       <c r="I104" s="26"/>
       <c r="J104" s="26"/>
       <c r="K104" s="26" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="L104" s="26" t="s">
-        <v>358</v>
+        <v>455</v>
       </c>
     </row>
     <row r="105" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -4982,7 +4983,7 @@
       </c>
       <c r="B105" s="26"/>
       <c r="C105" s="26" t="s">
-        <v>346</v>
+        <v>198</v>
       </c>
       <c r="D105" s="26" t="s">
         <v>4</v>
@@ -4994,10 +4995,10 @@
       <c r="I105" s="26"/>
       <c r="J105" s="26"/>
       <c r="K105" s="26" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="L105" s="26" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
     </row>
     <row r="106" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -5006,7 +5007,7 @@
       </c>
       <c r="B106" s="26"/>
       <c r="C106" s="26" t="s">
-        <v>430</v>
+        <v>342</v>
       </c>
       <c r="D106" s="26" t="s">
         <v>2</v>
@@ -5018,10 +5019,10 @@
       <c r="I106" s="26"/>
       <c r="J106" s="26"/>
       <c r="K106" s="26" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="L106" s="26" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="107" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -5030,10 +5031,10 @@
       </c>
       <c r="B107" s="26"/>
       <c r="C107" s="26" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="D107" s="26" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E107" s="26"/>
       <c r="F107" s="26"/>
@@ -5042,10 +5043,10 @@
       <c r="I107" s="26"/>
       <c r="J107" s="26"/>
       <c r="K107" s="26" t="s">
-        <v>349</v>
+        <v>436</v>
       </c>
       <c r="L107" s="26" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="108" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -5054,10 +5055,10 @@
       </c>
       <c r="B108" s="26"/>
       <c r="C108" s="26" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D108" s="26" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E108" s="26"/>
       <c r="F108" s="26"/>
@@ -5066,10 +5067,10 @@
       <c r="I108" s="26"/>
       <c r="J108" s="26"/>
       <c r="K108" s="26" t="s">
-        <v>454</v>
+        <v>435</v>
       </c>
       <c r="L108" s="26" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="109" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -5078,10 +5079,10 @@
       </c>
       <c r="B109" s="26"/>
       <c r="C109" s="26" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D109" s="26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E109" s="26"/>
       <c r="F109" s="26"/>
@@ -5090,9 +5091,11 @@
       <c r="I109" s="26"/>
       <c r="J109" s="26"/>
       <c r="K109" s="26" t="s">
-        <v>431</v>
-      </c>
-      <c r="L109" s="26"/>
+        <v>430</v>
+      </c>
+      <c r="L109" s="26" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="110" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="26" t="s">
@@ -5100,128 +5103,114 @@
       </c>
       <c r="B110" s="26"/>
       <c r="C110" s="26" t="s">
-        <v>141</v>
+        <v>349</v>
       </c>
       <c r="D110" s="26" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E110" s="26"/>
-      <c r="F110" s="26" t="s">
-        <v>122</v>
-      </c>
+      <c r="F110" s="26"/>
       <c r="G110" s="26"/>
-      <c r="H110" s="26" t="s">
-        <v>126</v>
-      </c>
+      <c r="H110" s="26"/>
       <c r="I110" s="26"/>
       <c r="J110" s="26"/>
-      <c r="K110" s="26"/>
+      <c r="K110" s="26" t="s">
+        <v>349</v>
+      </c>
       <c r="L110" s="26" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="B111" s="26"/>
+      <c r="C111" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="D111" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E111" s="26"/>
+      <c r="F111" s="26"/>
+      <c r="G111" s="26"/>
+      <c r="H111" s="26"/>
+      <c r="I111" s="26"/>
+      <c r="J111" s="26"/>
+      <c r="K111" s="26" t="s">
+        <v>454</v>
+      </c>
+      <c r="L111" s="26" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="B112" s="26"/>
+      <c r="C112" s="26" t="s">
+        <v>431</v>
+      </c>
+      <c r="D112" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E112" s="26"/>
+      <c r="F112" s="26"/>
+      <c r="G112" s="26"/>
+      <c r="H112" s="26"/>
+      <c r="I112" s="26"/>
+      <c r="J112" s="26"/>
+      <c r="K112" s="26" t="s">
+        <v>431</v>
+      </c>
+      <c r="L112" s="26"/>
+    </row>
+    <row r="113" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="B113" s="26"/>
+      <c r="C113" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="D113" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E113" s="26"/>
+      <c r="F113" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="G113" s="26"/>
+      <c r="H113" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="I113" s="26"/>
+      <c r="J113" s="26"/>
+      <c r="K113" s="26"/>
+      <c r="L113" s="26" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="111" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="24" t="s">
+    <row r="114" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="B111" s="24"/>
-      <c r="C111" s="24"/>
-      <c r="D111" s="24"/>
-      <c r="E111" s="24"/>
-      <c r="F111" s="24"/>
-      <c r="G111" s="24"/>
-      <c r="H111" s="24"/>
-      <c r="I111" s="24"/>
-      <c r="J111" s="24" t="s">
+      <c r="B114" s="24"/>
+      <c r="C114" s="24"/>
+      <c r="D114" s="24"/>
+      <c r="E114" s="24"/>
+      <c r="F114" s="24"/>
+      <c r="G114" s="24"/>
+      <c r="H114" s="24"/>
+      <c r="I114" s="24"/>
+      <c r="J114" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="K111" s="24"/>
-      <c r="L111" s="24" t="s">
+      <c r="K114" s="24"/>
+      <c r="L114" s="24" t="s">
         <v>362</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="B112" s="9"/>
-      <c r="C112" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D112" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E112" s="9">
-        <v>1</v>
-      </c>
-      <c r="F112" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="G112" s="9"/>
-      <c r="H112" s="9"/>
-      <c r="I112" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J112" s="9" t="s">
-        <v>399</v>
-      </c>
-      <c r="K112" s="9"/>
-      <c r="L112" s="9" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="113" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="B113" s="9"/>
-      <c r="C113" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="D113" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E113" s="9">
-        <v>1</v>
-      </c>
-      <c r="F113" s="9"/>
-      <c r="G113" s="9"/>
-      <c r="H113" s="9"/>
-      <c r="I113" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J113" s="9" t="s">
-        <v>396</v>
-      </c>
-      <c r="K113" s="9"/>
-      <c r="L113" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="114" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="B114" s="9"/>
-      <c r="C114" s="9" t="s">
-        <v>497</v>
-      </c>
-      <c r="D114" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E114" s="9"/>
-      <c r="F114" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="G114" s="9"/>
-      <c r="H114" s="9"/>
-      <c r="I114" s="9"/>
-      <c r="J114" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="K114" s="9"/>
-      <c r="L114" s="9" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="115" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -5230,24 +5219,28 @@
       </c>
       <c r="B115" s="9"/>
       <c r="C115" s="9" t="s">
-        <v>496</v>
+        <v>109</v>
       </c>
       <c r="D115" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E115" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="E115" s="9">
+        <v>1</v>
+      </c>
       <c r="F115" s="9" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G115" s="9"/>
       <c r="H115" s="9"/>
-      <c r="I115" s="9"/>
+      <c r="I115" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="J115" s="9" t="s">
-        <v>464</v>
+        <v>399</v>
       </c>
       <c r="K115" s="9"/>
       <c r="L115" s="9" t="s">
-        <v>364</v>
+        <v>328</v>
       </c>
     </row>
     <row r="116" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -5256,24 +5249,26 @@
       </c>
       <c r="B116" s="9"/>
       <c r="C116" s="9" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E116" s="9"/>
+        <v>2</v>
+      </c>
+      <c r="E116" s="9">
+        <v>1</v>
+      </c>
       <c r="F116" s="9"/>
       <c r="G116" s="9"/>
       <c r="H116" s="9"/>
-      <c r="I116" s="9"/>
+      <c r="I116" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="J116" s="9" t="s">
-        <v>386</v>
-      </c>
-      <c r="K116" s="9" t="s">
-        <v>432</v>
-      </c>
+        <v>396</v>
+      </c>
+      <c r="K116" s="9"/>
       <c r="L116" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="117" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -5282,109 +5277,128 @@
       </c>
       <c r="B117" s="9"/>
       <c r="C117" s="9" t="s">
-        <v>1</v>
+        <v>497</v>
       </c>
       <c r="D117" s="9" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E117" s="9"/>
-      <c r="F117" s="9"/>
+      <c r="F117" s="9" t="s">
+        <v>136</v>
+      </c>
       <c r="G117" s="9"/>
       <c r="H117" s="9"/>
       <c r="I117" s="9"/>
       <c r="J117" s="9" t="s">
-        <v>384</v>
+        <v>397</v>
       </c>
       <c r="K117" s="9"/>
       <c r="L117" s="9" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="B118" s="9"/>
+      <c r="C118" s="9" t="s">
+        <v>496</v>
+      </c>
+      <c r="D118" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E118" s="9"/>
+      <c r="F118" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="G118" s="9"/>
+      <c r="H118" s="9"/>
+      <c r="I118" s="9"/>
+      <c r="J118" s="9" t="s">
+        <v>464</v>
+      </c>
+      <c r="K118" s="9"/>
+      <c r="L118" s="9" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="B119" s="9"/>
+      <c r="C119" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D119" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E119" s="9"/>
+      <c r="F119" s="9"/>
+      <c r="G119" s="9"/>
+      <c r="H119" s="9"/>
+      <c r="I119" s="9"/>
+      <c r="J119" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="K119" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="L119" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="B120" s="9"/>
+      <c r="C120" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D120" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E120" s="9"/>
+      <c r="F120" s="9"/>
+      <c r="G120" s="9"/>
+      <c r="H120" s="9"/>
+      <c r="I120" s="9"/>
+      <c r="J120" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="K120" s="9"/>
+      <c r="L120" s="9" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="118" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="28" t="s">
+    <row r="121" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="L118" s="28" t="s">
+      <c r="L121" s="28" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="119" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C119" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D119" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E119" s="8">
-        <v>1</v>
-      </c>
-      <c r="F119" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="I119" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C120" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D120" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E120" s="8">
-        <v>1</v>
-      </c>
-      <c r="I120" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B121" s="8"/>
-      <c r="C121" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D121" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E121" s="8"/>
-      <c r="F121" s="8"/>
-      <c r="G121" s="8"/>
-      <c r="H121" s="8"/>
-      <c r="I121" s="8"/>
-      <c r="J121" s="8"/>
-      <c r="K121" s="8"/>
-      <c r="L121" s="8"/>
-    </row>
-    <row r="122" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B122" s="8"/>
       <c r="C122" s="8" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E122" s="8"/>
-      <c r="F122" s="8"/>
-      <c r="G122" s="8"/>
-      <c r="H122" s="8"/>
-      <c r="I122" s="8"/>
-      <c r="J122" s="8"/>
-      <c r="K122" s="8"/>
-      <c r="L122" s="8" t="s">
-        <v>370</v>
+        <v>16</v>
+      </c>
+      <c r="E122" s="8">
+        <v>1</v>
+      </c>
+      <c r="F122" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="I122" s="8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -5392,13 +5406,16 @@
         <v>19</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="L123" s="8" t="s">
-        <v>371</v>
+        <v>2</v>
+      </c>
+      <c r="E123" s="8">
+        <v>1</v>
+      </c>
+      <c r="I123" s="8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -5407,23 +5424,19 @@
       </c>
       <c r="B124" s="8"/>
       <c r="C124" s="8" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E124" s="8"/>
-      <c r="F124" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="F124" s="8"/>
       <c r="G124" s="8"/>
       <c r="H124" s="8"/>
       <c r="I124" s="8"/>
       <c r="J124" s="8"/>
       <c r="K124" s="8"/>
-      <c r="L124" s="8" t="s">
-        <v>373</v>
-      </c>
+      <c r="L124" s="8"/>
     </row>
     <row r="125" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="8" t="s">
@@ -5431,44 +5444,34 @@
       </c>
       <c r="B125" s="8"/>
       <c r="C125" s="8" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E125" s="8"/>
-      <c r="F125" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="F125" s="8"/>
       <c r="G125" s="8"/>
       <c r="H125" s="8"/>
       <c r="I125" s="8"/>
       <c r="J125" s="8"/>
       <c r="K125" s="8"/>
       <c r="L125" s="8" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="126" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B126" s="8"/>
       <c r="C126" s="8" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="D126" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E126" s="8"/>
-      <c r="F126" s="8"/>
-      <c r="G126" s="8"/>
-      <c r="H126" s="8"/>
-      <c r="I126" s="8"/>
-      <c r="J126" s="8"/>
-      <c r="K126" s="8"/>
       <c r="L126" s="8" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
     <row r="127" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -5477,132 +5480,128 @@
       </c>
       <c r="B127" s="8"/>
       <c r="C127" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E127" s="8"/>
       <c r="F127" s="8" t="s">
-        <v>491</v>
-      </c>
-      <c r="G127" s="8" t="s">
-        <v>109</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G127" s="8"/>
       <c r="H127" s="8"/>
       <c r="I127" s="8"/>
       <c r="J127" s="8"/>
       <c r="K127" s="8"/>
       <c r="L127" s="8" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="128" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B128" s="8"/>
       <c r="C128" s="8" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E128" s="8"/>
-      <c r="F128" s="8"/>
+      <c r="F128" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="G128" s="8"/>
       <c r="H128" s="8"/>
       <c r="I128" s="8"/>
       <c r="J128" s="8"/>
       <c r="K128" s="8"/>
       <c r="L128" s="8" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="129" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="28" t="s">
-        <v>491</v>
-      </c>
-      <c r="K129" s="28" t="s">
-        <v>446</v>
-      </c>
-      <c r="L129" s="28" t="s">
-        <v>376</v>
+        <v>372</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B129" s="8"/>
+      <c r="C129" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D129" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E129" s="8"/>
+      <c r="F129" s="8"/>
+      <c r="G129" s="8"/>
+      <c r="H129" s="8"/>
+      <c r="I129" s="8"/>
+      <c r="J129" s="8"/>
+      <c r="K129" s="8"/>
+      <c r="L129" s="8" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="130" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="8" t="s">
-        <v>491</v>
+        <v>19</v>
       </c>
       <c r="B130" s="8"/>
       <c r="C130" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D130" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E130" s="8"/>
+      <c r="F130" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="G130" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="D130" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E130" s="8">
-        <v>1</v>
-      </c>
-      <c r="F130" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="G130" s="8"/>
       <c r="H130" s="8"/>
-      <c r="I130" s="8" t="b">
-        <v>1</v>
-      </c>
+      <c r="I130" s="8"/>
       <c r="J130" s="8"/>
       <c r="K130" s="8"/>
       <c r="L130" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="131" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="8" t="s">
-        <v>491</v>
+        <v>19</v>
       </c>
       <c r="B131" s="8"/>
       <c r="C131" s="8" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E131" s="8">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E131" s="8"/>
       <c r="F131" s="8"/>
       <c r="G131" s="8"/>
       <c r="H131" s="8"/>
-      <c r="I131" s="8" t="b">
-        <v>1</v>
-      </c>
+      <c r="I131" s="8"/>
       <c r="J131" s="8"/>
       <c r="K131" s="8"/>
       <c r="L131" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="132" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="8" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="28" t="s">
         <v>491</v>
       </c>
-      <c r="B132" s="8"/>
-      <c r="C132" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D132" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E132" s="8"/>
-      <c r="F132" s="8"/>
-      <c r="G132" s="8"/>
-      <c r="H132" s="8"/>
-      <c r="I132" s="8"/>
-      <c r="J132" s="8"/>
-      <c r="K132" s="8"/>
-      <c r="L132" s="8"/>
+      <c r="K132" s="28" t="s">
+        <v>446</v>
+      </c>
+      <c r="L132" s="28" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="133" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A133" s="8" t="s">
@@ -5610,64 +5609,138 @@
       </c>
       <c r="B133" s="8"/>
       <c r="C133" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D133" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E133" s="8">
         <v>1</v>
       </c>
-      <c r="D133" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E133" s="8"/>
-      <c r="F133" s="8"/>
+      <c r="F133" s="8" t="s">
+        <v>122</v>
+      </c>
       <c r="G133" s="8"/>
       <c r="H133" s="8"/>
-      <c r="I133" s="8"/>
+      <c r="I133" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="J133" s="8"/>
       <c r="K133" s="8"/>
-      <c r="L133" s="8"/>
-    </row>
-    <row r="134" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L133" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="8" t="s">
         <v>491</v>
       </c>
+      <c r="B134" s="8"/>
       <c r="C134" s="8" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F134" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="135" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="E134" s="8">
+        <v>1</v>
+      </c>
+      <c r="F134" s="8"/>
+      <c r="G134" s="8"/>
+      <c r="H134" s="8"/>
+      <c r="I134" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J134" s="8"/>
+      <c r="K134" s="8"/>
+      <c r="L134" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="8" t="s">
         <v>491</v>
       </c>
+      <c r="B135" s="8"/>
       <c r="C135" s="8" t="s">
-        <v>493</v>
+        <v>5</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F135" s="8" t="s">
-        <v>561</v>
-      </c>
-      <c r="L135" s="8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="136" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="E135" s="8"/>
+      <c r="F135" s="8"/>
+      <c r="G135" s="8"/>
+      <c r="H135" s="8"/>
+      <c r="I135" s="8"/>
+      <c r="J135" s="8"/>
+      <c r="K135" s="8"/>
+      <c r="L135" s="8"/>
+    </row>
+    <row r="136" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="8" t="s">
         <v>491</v>
       </c>
+      <c r="B136" s="8"/>
       <c r="C136" s="8" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="D136" s="8" t="s">
         <v>3</v>
       </c>
+      <c r="E136" s="8"/>
+      <c r="F136" s="8"/>
+      <c r="G136" s="8"/>
+      <c r="H136" s="8"/>
+      <c r="I136" s="8"/>
+      <c r="J136" s="8"/>
+      <c r="K136" s="8"/>
+      <c r="L136" s="8"/>
+    </row>
+    <row r="137" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="C137" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D137" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F137" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="C138" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="D138" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F138" s="8" t="s">
+        <v>561</v>
+      </c>
+      <c r="L138" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="C139" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D139" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M97" xr:uid="{05A83487-31A5-894A-B1C5-9D57C8ECFC86}"/>
+  <autoFilter ref="A1:M100" xr:uid="{05A83487-31A5-894A-B1C5-9D57C8ECFC86}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>